<commit_message>
Use dropdown for dob
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="543">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -819,6 +819,450 @@
   </si>
   <si>
     <t xml:space="preserve">Traditional_medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1921</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_1920</t>
   </si>
   <si>
     <t xml:space="preserve">valuesList</t>
@@ -1521,7 +1965,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.87890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -2562,11 +3006,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1006"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.87890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
@@ -3943,13 +4387,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C255"/>
+  <dimension ref="A1:C400"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A188" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A207" activeCellId="0" sqref="A207"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A200" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A256" activeCellId="0" sqref="A256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -6759,6 +7203,1601 @@
       </c>
       <c r="C255" s="0" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C256" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C257" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C258" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C259" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C260" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C261" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B264" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C264" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C265" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C266" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C267" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C268" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B269" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C269" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B270" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C270" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C271" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C272" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B273" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C273" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B274" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C274" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B275" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C275" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C277" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C278" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C279" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C280" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C281" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B282" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C282" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C283" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C284" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C285" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C286" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C287" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C288" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B289" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C289" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C290" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C291" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C292" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C293" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C294" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B295" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C295" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B296" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C296" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B297" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C297" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B298" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B299" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C299" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B300" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C300" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B301" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C301" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B302" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C302" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B303" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C303" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B304" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C304" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B305" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C305" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B306" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C306" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B307" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C307" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B308" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C308" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B309" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C309" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B310" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C310" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B311" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C311" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B312" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C312" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B313" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C313" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B314" s="0" t="n">
+        <v>2006</v>
+      </c>
+      <c r="C314" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B315" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C315" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B316" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B317" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C317" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B318" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C318" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B319" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C319" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B320" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C320" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B321" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="C321" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B322" s="0" t="n">
+        <v>1998</v>
+      </c>
+      <c r="C322" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B323" s="0" t="n">
+        <v>1997</v>
+      </c>
+      <c r="C323" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B324" s="0" t="n">
+        <v>1996</v>
+      </c>
+      <c r="C324" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B325" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="C325" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B326" s="0" t="n">
+        <v>1994</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B327" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B328" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B329" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="C329" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B330" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="C330" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B331" s="0" t="n">
+        <v>1989</v>
+      </c>
+      <c r="C331" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B332" s="0" t="n">
+        <v>1988</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B333" s="0" t="n">
+        <v>1987</v>
+      </c>
+      <c r="C333" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B334" s="0" t="n">
+        <v>1986</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B335" s="0" t="n">
+        <v>1985</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B336" s="0" t="n">
+        <v>1984</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B337" s="0" t="n">
+        <v>1983</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B338" s="0" t="n">
+        <v>1982</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B339" s="0" t="n">
+        <v>1981</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B340" s="0" t="n">
+        <v>1980</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B341" s="0" t="n">
+        <v>1979</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B342" s="0" t="n">
+        <v>1978</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B343" s="0" t="n">
+        <v>1977</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B344" s="0" t="n">
+        <v>1976</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B345" s="0" t="n">
+        <v>1975</v>
+      </c>
+      <c r="C345" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B346" s="0" t="n">
+        <v>1974</v>
+      </c>
+      <c r="C346" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B347" s="0" t="n">
+        <v>1973</v>
+      </c>
+      <c r="C347" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B348" s="0" t="n">
+        <v>1972</v>
+      </c>
+      <c r="C348" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B349" s="0" t="n">
+        <v>1971</v>
+      </c>
+      <c r="C349" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B350" s="0" t="n">
+        <v>1970</v>
+      </c>
+      <c r="C350" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B351" s="0" t="n">
+        <v>1969</v>
+      </c>
+      <c r="C351" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B352" s="0" t="n">
+        <v>1968</v>
+      </c>
+      <c r="C352" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B353" s="0" t="n">
+        <v>1967</v>
+      </c>
+      <c r="C353" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B354" s="0" t="n">
+        <v>1966</v>
+      </c>
+      <c r="C354" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B355" s="0" t="n">
+        <v>1965</v>
+      </c>
+      <c r="C355" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B356" s="0" t="n">
+        <v>1964</v>
+      </c>
+      <c r="C356" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B357" s="0" t="n">
+        <v>1963</v>
+      </c>
+      <c r="C357" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B358" s="0" t="n">
+        <v>1962</v>
+      </c>
+      <c r="C358" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B359" s="0" t="n">
+        <v>1961</v>
+      </c>
+      <c r="C359" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B360" s="0" t="n">
+        <v>1960</v>
+      </c>
+      <c r="C360" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B361" s="0" t="n">
+        <v>1959</v>
+      </c>
+      <c r="C361" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B362" s="0" t="n">
+        <v>1958</v>
+      </c>
+      <c r="C362" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B363" s="0" t="n">
+        <v>1957</v>
+      </c>
+      <c r="C363" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B364" s="0" t="n">
+        <v>1956</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B365" s="0" t="n">
+        <v>1955</v>
+      </c>
+      <c r="C365" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B366" s="0" t="n">
+        <v>1954</v>
+      </c>
+      <c r="C366" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B367" s="0" t="n">
+        <v>1953</v>
+      </c>
+      <c r="C367" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B368" s="0" t="n">
+        <v>1952</v>
+      </c>
+      <c r="C368" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B369" s="0" t="n">
+        <v>1951</v>
+      </c>
+      <c r="C369" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B370" s="0" t="n">
+        <v>1950</v>
+      </c>
+      <c r="C370" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B371" s="0" t="n">
+        <v>1949</v>
+      </c>
+      <c r="C371" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B372" s="0" t="n">
+        <v>1948</v>
+      </c>
+      <c r="C372" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B373" s="0" t="n">
+        <v>1947</v>
+      </c>
+      <c r="C373" s="0" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B374" s="0" t="n">
+        <v>1946</v>
+      </c>
+      <c r="C374" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B375" s="0" t="n">
+        <v>1945</v>
+      </c>
+      <c r="C375" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B376" s="0" t="n">
+        <v>1944</v>
+      </c>
+      <c r="C376" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B377" s="0" t="n">
+        <v>1943</v>
+      </c>
+      <c r="C377" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B378" s="0" t="n">
+        <v>1942</v>
+      </c>
+      <c r="C378" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B379" s="0" t="n">
+        <v>1941</v>
+      </c>
+      <c r="C379" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B380" s="0" t="n">
+        <v>1940</v>
+      </c>
+      <c r="C380" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B381" s="0" t="n">
+        <v>1939</v>
+      </c>
+      <c r="C381" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B382" s="0" t="n">
+        <v>1938</v>
+      </c>
+      <c r="C382" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B383" s="0" t="n">
+        <v>1937</v>
+      </c>
+      <c r="C383" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B384" s="0" t="n">
+        <v>1936</v>
+      </c>
+      <c r="C384" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B385" s="0" t="n">
+        <v>1935</v>
+      </c>
+      <c r="C385" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B386" s="0" t="n">
+        <v>1934</v>
+      </c>
+      <c r="C386" s="0" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B387" s="0" t="n">
+        <v>1933</v>
+      </c>
+      <c r="C387" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B388" s="0" t="n">
+        <v>1932</v>
+      </c>
+      <c r="C388" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B389" s="0" t="n">
+        <v>1931</v>
+      </c>
+      <c r="C389" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B390" s="0" t="n">
+        <v>1930</v>
+      </c>
+      <c r="C390" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B391" s="0" t="n">
+        <v>1929</v>
+      </c>
+      <c r="C391" s="0" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B392" s="0" t="n">
+        <v>1928</v>
+      </c>
+      <c r="C392" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B393" s="0" t="n">
+        <v>1927</v>
+      </c>
+      <c r="C393" s="0" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B394" s="0" t="n">
+        <v>1926</v>
+      </c>
+      <c r="C394" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B395" s="0" t="n">
+        <v>1925</v>
+      </c>
+      <c r="C395" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B396" s="0" t="n">
+        <v>1924</v>
+      </c>
+      <c r="C396" s="0" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B397" s="0" t="n">
+        <v>1923</v>
+      </c>
+      <c r="C397" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B398" s="0" t="n">
+        <v>1922</v>
+      </c>
+      <c r="C398" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B399" s="0" t="n">
+        <v>1921</v>
+      </c>
+      <c r="C399" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B400" s="0" t="n">
+        <v>1920</v>
+      </c>
+      <c r="C400" s="0" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -6783,7 +8822,7 @@
       <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -6804,48 +8843,48 @@
         <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>265</v>
+        <v>413</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>266</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>267</v>
+        <v>415</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>268</v>
+        <v>416</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>269</v>
+        <v>417</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="8" t="s">
-        <v>270</v>
+        <v>418</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>269</v>
+        <v>417</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
-        <v>271</v>
+        <v>419</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>269</v>
+        <v>417</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>272</v>
+        <v>420</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>269</v>
+        <v>417</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>1</v>
@@ -6853,100 +8892,100 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8" t="s">
-        <v>273</v>
+        <v>421</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
-        <v>275</v>
+        <v>423</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
-        <v>276</v>
+        <v>424</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
-        <v>277</v>
+        <v>425</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>278</v>
+        <v>426</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
-        <v>279</v>
+        <v>427</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>280</v>
+        <v>428</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>281</v>
+        <v>429</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
-        <v>283</v>
+        <v>431</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
-        <v>284</v>
+        <v>432</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="9" t="s">
-        <v>285</v>
+        <v>433</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>29</v>
@@ -6958,16 +8997,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
-        <v>286</v>
+        <v>434</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
-        <v>287</v>
+        <v>435</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>29</v>
@@ -6979,16 +9018,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="9" t="s">
-        <v>288</v>
+        <v>436</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
-        <v>289</v>
+        <v>437</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
@@ -7000,16 +9039,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
-        <v>290</v>
+        <v>438</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="9" t="s">
-        <v>291</v>
+        <v>439</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>29</v>
@@ -7045,16 +9084,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
-        <v>292</v>
+        <v>440</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>293</v>
+        <v>441</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>24</v>
@@ -7078,16 +9117,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10" t="s">
-        <v>294</v>
+        <v>442</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>295</v>
+        <v>443</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>22</v>
@@ -7123,7 +9162,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>296</v>
+        <v>444</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>170</v>
@@ -7138,16 +9177,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>297</v>
+        <v>445</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>298</v>
+        <v>446</v>
       </c>
       <c r="E33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="s">
-        <v>299</v>
+        <v>447</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>29</v>
@@ -7159,25 +9198,25 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="s">
-        <v>300</v>
+        <v>448</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>298</v>
+        <v>446</v>
       </c>
       <c r="E35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="11" t="s">
-        <v>301</v>
+        <v>449</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="11" t="s">
-        <v>302</v>
+        <v>450</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>22</v>
@@ -7189,7 +9228,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="11" t="s">
-        <v>303</v>
+        <v>451</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>22</v>
@@ -7201,10 +9240,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>304</v>
+        <v>452</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>305</v>
+        <v>453</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>22</v>
@@ -7216,25 +9255,25 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="12" t="s">
-        <v>306</v>
+        <v>454</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>298</v>
+        <v>446</v>
       </c>
       <c r="E40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="12" t="s">
-        <v>307</v>
+        <v>455</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="12" t="s">
-        <v>308</v>
+        <v>456</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>22</v>
@@ -7246,7 +9285,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="12" t="s">
-        <v>309</v>
+        <v>457</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>22</v>
@@ -7258,7 +9297,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="12" t="s">
-        <v>310</v>
+        <v>458</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>22</v>
@@ -7270,7 +9309,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="12" t="s">
-        <v>311</v>
+        <v>459</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>29</v>
@@ -7282,10 +9321,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>312</v>
+        <v>460</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>313</v>
+        <v>461</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
@@ -7297,7 +9336,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
-        <v>314</v>
+        <v>462</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>29</v>
@@ -7309,19 +9348,19 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>315</v>
+        <v>463</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>316</v>
+        <v>464</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
-        <v>317</v>
+        <v>465</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>29</v>
@@ -7333,7 +9372,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
-        <v>318</v>
+        <v>466</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>22</v>
@@ -7345,16 +9384,16 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>319</v>
+        <v>467</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>320</v>
+        <v>468</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>29</v>
@@ -7366,7 +9405,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
-        <v>321</v>
+        <v>469</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>29</v>
@@ -7378,16 +9417,16 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
-        <v>322</v>
+        <v>470</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
-        <v>323</v>
+        <v>471</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>22</v>
@@ -7399,10 +9438,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>324</v>
+        <v>472</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>325</v>
+        <v>473</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>22</v>
@@ -7414,7 +9453,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="14" t="s">
-        <v>326</v>
+        <v>474</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>22</v>
@@ -7426,7 +9465,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="14" t="s">
-        <v>327</v>
+        <v>475</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>22</v>
@@ -7438,16 +9477,16 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="14" t="s">
-        <v>328</v>
+        <v>476</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>329</v>
+        <v>477</v>
       </c>
       <c r="E59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="14" t="s">
-        <v>330</v>
+        <v>478</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>22</v>
@@ -7459,25 +9498,25 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="14" t="s">
-        <v>331</v>
+        <v>479</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>329</v>
+        <v>477</v>
       </c>
       <c r="E61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="14" t="s">
-        <v>332</v>
+        <v>480</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>329</v>
+        <v>477</v>
       </c>
       <c r="E62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="14" t="s">
-        <v>333</v>
+        <v>481</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>22</v>
@@ -7489,7 +9528,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="14" t="s">
-        <v>334</v>
+        <v>482</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>22</v>
@@ -7513,19 +9552,19 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="14" t="s">
-        <v>335</v>
+        <v>483</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>336</v>
+        <v>484</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>337</v>
+        <v>485</v>
       </c>
       <c r="E66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="14" t="s">
-        <v>338</v>
+        <v>486</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>29</v>
@@ -7537,7 +9576,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="14" t="s">
-        <v>339</v>
+        <v>487</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>29</v>
@@ -7549,16 +9588,16 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="14" t="s">
-        <v>340</v>
+        <v>488</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="14" t="s">
-        <v>341</v>
+        <v>489</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>22</v>
@@ -7570,7 +9609,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="14" t="s">
-        <v>342</v>
+        <v>490</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>29</v>
@@ -7582,16 +9621,16 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="14" t="s">
-        <v>343</v>
+        <v>491</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="14" t="s">
-        <v>344</v>
+        <v>492</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>29</v>
@@ -7603,16 +9642,16 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="14" t="s">
-        <v>345</v>
+        <v>493</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E74" s="7"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="14" t="s">
-        <v>346</v>
+        <v>494</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>22</v>
@@ -7624,7 +9663,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="14" t="s">
-        <v>347</v>
+        <v>495</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>29</v>
@@ -7636,16 +9675,16 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="14" t="s">
-        <v>348</v>
+        <v>496</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>282</v>
+        <v>430</v>
       </c>
       <c r="E77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="14" t="s">
-        <v>349</v>
+        <v>497</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>22</v>
@@ -7657,7 +9696,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="14" t="s">
-        <v>350</v>
+        <v>498</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>22</v>
@@ -7669,7 +9708,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="14" t="s">
-        <v>351</v>
+        <v>499</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>22</v>
@@ -7681,7 +9720,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="14" t="s">
-        <v>352</v>
+        <v>500</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>22</v>
@@ -7693,7 +9732,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="14" t="s">
-        <v>353</v>
+        <v>501</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>29</v>
@@ -7705,7 +9744,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="14" t="s">
-        <v>354</v>
+        <v>502</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>29</v>
@@ -7717,7 +9756,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="14" t="s">
-        <v>355</v>
+        <v>503</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>22</v>
@@ -7729,7 +9768,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="14" t="s">
-        <v>356</v>
+        <v>504</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>22</v>
@@ -7741,7 +9780,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="14" t="s">
-        <v>357</v>
+        <v>505</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>22</v>
@@ -7753,7 +9792,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="14" t="s">
-        <v>358</v>
+        <v>506</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>22</v>
@@ -7765,7 +9804,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="14" t="s">
-        <v>359</v>
+        <v>507</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>22</v>
@@ -7777,7 +9816,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="14" t="s">
-        <v>360</v>
+        <v>508</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>22</v>
@@ -7789,7 +9828,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="14" t="s">
-        <v>361</v>
+        <v>509</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>22</v>
@@ -7801,7 +9840,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
-        <v>362</v>
+        <v>510</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>22</v>
@@ -7813,16 +9852,16 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="14" t="s">
-        <v>363</v>
+        <v>511</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E92" s="7"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="14" t="s">
-        <v>364</v>
+        <v>512</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>22</v>
@@ -7846,7 +9885,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="14" t="s">
-        <v>365</v>
+        <v>513</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>22</v>
@@ -7858,7 +9897,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="14" t="s">
-        <v>366</v>
+        <v>514</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>29</v>
@@ -7870,7 +9909,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="14" t="s">
-        <v>367</v>
+        <v>515</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>22</v>
@@ -7882,7 +9921,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="14" t="s">
-        <v>368</v>
+        <v>516</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>22</v>
@@ -7894,7 +9933,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="14" t="s">
-        <v>369</v>
+        <v>517</v>
       </c>
       <c r="C99" s="14" t="s">
         <v>29</v>
@@ -7906,7 +9945,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="14" t="s">
-        <v>370</v>
+        <v>518</v>
       </c>
       <c r="C100" s="14" t="s">
         <v>22</v>
@@ -7930,7 +9969,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="14" t="s">
-        <v>371</v>
+        <v>519</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>22</v>
@@ -7942,10 +9981,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="14" t="s">
-        <v>372</v>
+        <v>520</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="E103" s="7"/>
     </row>
@@ -9947,11 +11986,11 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.87890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.01"/>
@@ -9964,71 +12003,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>373</v>
+        <v>521</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>374</v>
+        <v>522</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>375</v>
+        <v>523</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>376</v>
+        <v>524</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>377</v>
+        <v>525</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>378</v>
+        <v>526</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>379</v>
+        <v>527</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>380</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>381</v>
+        <v>529</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>382</v>
+        <v>530</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>383</v>
+        <v>531</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210207001</v>
+        <v>20210221001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>384</v>
+        <v>532</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>385</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>386</v>
+        <v>534</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>387</v>
+        <v>535</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>387</v>
+        <v>535</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>387</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>388</v>
+        <v>536</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -10036,44 +12075,44 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>389</v>
+        <v>537</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>390</v>
+        <v>538</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>390</v>
+        <v>538</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>390</v>
+        <v>538</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>391</v>
+        <v>539</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>392</v>
+        <v>540</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>392</v>
+        <v>540</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>392</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>393</v>
+        <v>541</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>394</v>
+        <v>542</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>394</v>
+        <v>542</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>394</v>
+        <v>542</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Implement ExtId assignment for non-resident/deceased
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="549">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1265,12 +1265,21 @@
     <t xml:space="preserve">year_1920</t>
   </si>
   <si>
+    <t xml:space="preserve">elementType</t>
+  </si>
+  <si>
     <t xml:space="preserve">valuesList</t>
   </si>
   <si>
     <t xml:space="preserve">isSessionVariable</t>
   </si>
   <si>
+    <t xml:space="preserve">properties.resident.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">properties.non_resident.type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assigned by household form</t>
   </si>
   <si>
@@ -1287,6 +1296,12 @@
   </si>
   <si>
     <t xml:space="preserve">id_candidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extIdObj</t>
   </si>
   <si>
     <t xml:space="preserve">form_status_hh_member</t>
@@ -1968,7 +1983,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.90625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.94921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -3013,7 +3028,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.90625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.94921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
@@ -4396,7 +4411,7 @@
       <selection pane="topLeft" activeCell="A256" activeCellId="0" sqref="A256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -8819,19 +8834,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E763"/>
+  <dimension ref="A1:H763"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.12"/>
   </cols>
   <sheetData>
@@ -8848,218 +8865,256 @@
       <c r="D1" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="0" t="s">
         <v>414</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="E2" s="7"/>
+        <v>420</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="8" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="E3" s="7"/>
+        <v>420</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>420</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>1</v>
+      <c r="H5" s="0" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E6" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E7" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E8" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="E12" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="E13" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="E14" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="E15" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="9" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="E17" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="9" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="9" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
@@ -9068,10 +9123,11 @@
       <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
@@ -9080,23 +9136,25 @@
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>430</v>
-      </c>
-      <c r="E25" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>24</v>
@@ -9104,10 +9162,11 @@
       <c r="C26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="10" t="s">
@@ -9116,28 +9175,31 @@
       <c r="C27" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="D27" s="10"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="E28" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="10" t="s">
@@ -9146,10 +9208,11 @@
       <c r="C30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="10"/>
+      <c r="E30" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="10" t="s">
@@ -9158,14 +9221,15 @@
       <c r="C31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="10"/>
+      <c r="E31" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>170</v>
@@ -9173,373 +9237,406 @@
       <c r="C32" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="11"/>
+      <c r="E32" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="E33" s="7"/>
+        <v>451</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="11"/>
+      <c r="E34" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="E35" s="7"/>
+        <v>451</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="11" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="E36" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="11" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="11"/>
+      <c r="E37" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="11" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="11"/>
+      <c r="E38" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="12"/>
+      <c r="E39" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="12" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="E40" s="7"/>
+        <v>451</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="12" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>422</v>
-      </c>
-      <c r="E41" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="12" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="12"/>
+      <c r="E42" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="12" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="12" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="12" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="12"/>
+      <c r="E45" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="9"/>
+      <c r="E46" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="9"/>
+      <c r="E47" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="E48" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D48" s="13"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="13"/>
+      <c r="E49" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="13"/>
+      <c r="E50" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="E51" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="13"/>
+      <c r="E52" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="13"/>
+      <c r="E53" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="E54" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D54" s="13"/>
+      <c r="F54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="13"/>
+      <c r="E55" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="14"/>
+      <c r="E56" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="14" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="14"/>
+      <c r="E57" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="14" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="14"/>
+      <c r="E58" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="14" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="E59" s="7"/>
+        <v>482</v>
+      </c>
+      <c r="D59" s="14"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="14" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="14"/>
+      <c r="E60" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="14" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="E61" s="7"/>
+        <v>482</v>
+      </c>
+      <c r="D61" s="14"/>
+      <c r="F61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="14" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="E62" s="7"/>
+        <v>482</v>
+      </c>
+      <c r="D62" s="14"/>
+      <c r="F62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="14" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="14"/>
+      <c r="E63" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="14" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="14"/>
+      <c r="E64" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="14" t="s">
@@ -9548,331 +9645,360 @@
       <c r="C65" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="14"/>
+      <c r="E65" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="14" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>484</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E66" s="7"/>
+        <v>489</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="14" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="14"/>
+      <c r="E67" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="14" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" s="14"/>
+      <c r="E68" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="14" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="E69" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D69" s="14"/>
+      <c r="F69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="14" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="14"/>
+      <c r="E70" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="14" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="14"/>
+      <c r="E71" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="14" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="E72" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="F72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="14" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="14"/>
+      <c r="E73" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="14" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="E74" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D74" s="14"/>
+      <c r="F74" s="7"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="14" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" s="14"/>
+      <c r="E75" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="14" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" s="14"/>
+      <c r="E76" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="14" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="E77" s="7"/>
+        <v>435</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="F77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="14" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D78" s="0" t="s">
+      <c r="D78" s="14"/>
+      <c r="E78" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="14" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" s="14"/>
+      <c r="E79" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="14" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D80" s="0" t="s">
+      <c r="D80" s="14"/>
+      <c r="E80" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="14" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" s="14"/>
+      <c r="E81" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="14" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" s="14"/>
+      <c r="E82" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="14" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" s="14"/>
+      <c r="E83" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="14" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D84" s="0" t="s">
+      <c r="D84" s="14"/>
+      <c r="E84" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="14" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D85" s="0" t="s">
+      <c r="D85" s="14"/>
+      <c r="E85" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="14" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D86" s="0" t="s">
+      <c r="D86" s="14"/>
+      <c r="E86" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="14" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" s="14"/>
+      <c r="E87" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="14" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="14"/>
+      <c r="E88" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="14" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" s="14"/>
+      <c r="E89" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="14" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="D90" s="14"/>
+      <c r="E90" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" s="14"/>
+      <c r="E91" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="14" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>422</v>
-      </c>
-      <c r="E92" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D92" s="14"/>
+      <c r="F92" s="7"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="14" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D93" s="0" t="s">
+      <c r="D93" s="14"/>
+      <c r="E93" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="14" t="s">
@@ -9881,82 +10007,89 @@
       <c r="C94" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D94" s="0" t="s">
+      <c r="D94" s="14"/>
+      <c r="E94" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="14" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D95" s="0" t="s">
+      <c r="D95" s="14"/>
+      <c r="E95" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="14" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D96" s="0" t="s">
+      <c r="D96" s="14"/>
+      <c r="E96" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="14" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D97" s="0" t="s">
+      <c r="D97" s="14"/>
+      <c r="E97" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="14" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D98" s="0" t="s">
+      <c r="D98" s="14"/>
+      <c r="E98" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="14" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="C99" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D99" s="0" t="s">
+      <c r="D99" s="14"/>
+      <c r="E99" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="14" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="C100" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D100" s="0" t="s">
+      <c r="D100" s="14"/>
+      <c r="E100" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="14" t="s">
@@ -9965,2011 +10098,2014 @@
       <c r="C101" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D101" s="0" t="s">
+      <c r="D101" s="14"/>
+      <c r="E101" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="14" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D102" s="0" t="s">
+      <c r="D102" s="14"/>
+      <c r="E102" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="14" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>422</v>
-      </c>
-      <c r="E103" s="7"/>
+        <v>427</v>
+      </c>
+      <c r="D103" s="14"/>
+      <c r="F103" s="7"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E127" s="7"/>
+      <c r="F127" s="7"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E131" s="7"/>
+      <c r="F131" s="7"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E135" s="7"/>
+      <c r="F135" s="7"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E137" s="7"/>
+      <c r="F137" s="7"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E138" s="7"/>
+      <c r="F138" s="7"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E139" s="7"/>
+      <c r="F139" s="7"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E141" s="7"/>
+      <c r="F141" s="7"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E142" s="7"/>
+      <c r="F142" s="7"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E143" s="7"/>
+      <c r="F143" s="7"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E144" s="7"/>
+      <c r="F144" s="7"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E145" s="7"/>
+      <c r="F145" s="7"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E146" s="7"/>
+      <c r="F146" s="7"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E147" s="7"/>
+      <c r="F147" s="7"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E148" s="7"/>
+      <c r="F148" s="7"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E152" s="7"/>
+      <c r="F152" s="7"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E153" s="7"/>
+      <c r="F153" s="7"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E154" s="7"/>
+      <c r="F154" s="7"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E155" s="7"/>
+      <c r="F155" s="7"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E156" s="7"/>
+      <c r="F156" s="7"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E157" s="7"/>
+      <c r="F157" s="7"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E158" s="7"/>
+      <c r="F158" s="7"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E162" s="7"/>
+      <c r="F162" s="7"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E164" s="7"/>
+      <c r="F164" s="7"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E165" s="7"/>
+      <c r="F165" s="7"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E166" s="7"/>
+      <c r="F166" s="7"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E167" s="7"/>
+      <c r="F167" s="7"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E168" s="7"/>
+      <c r="F168" s="7"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E169" s="7"/>
+      <c r="F169" s="7"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E170" s="7"/>
+      <c r="F170" s="7"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E171" s="7"/>
+      <c r="F171" s="7"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E172" s="7"/>
+      <c r="F172" s="7"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E173" s="7"/>
+      <c r="F173" s="7"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E174" s="7"/>
+      <c r="F174" s="7"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E175" s="7"/>
+      <c r="F175" s="7"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E178" s="7"/>
+      <c r="F178" s="7"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E179" s="7"/>
+      <c r="F179" s="7"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E180" s="7"/>
+      <c r="F180" s="7"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E181" s="7"/>
+      <c r="F181" s="7"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E183" s="7"/>
+      <c r="F183" s="7"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E184" s="7"/>
+      <c r="F184" s="7"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E185" s="7"/>
+      <c r="F185" s="7"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E186" s="7"/>
+      <c r="F186" s="7"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E187" s="7"/>
+      <c r="F187" s="7"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E189" s="7"/>
+      <c r="F189" s="7"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E190" s="7"/>
+      <c r="F190" s="7"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E191" s="7"/>
+      <c r="F191" s="7"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E192" s="7"/>
+      <c r="F192" s="7"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E193" s="7"/>
+      <c r="F193" s="7"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E194" s="7"/>
+      <c r="F194" s="7"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E195" s="7"/>
+      <c r="F195" s="7"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E196" s="7"/>
+      <c r="F196" s="7"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E197" s="7"/>
+      <c r="F197" s="7"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E198" s="7"/>
+      <c r="F198" s="7"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E199" s="7"/>
+      <c r="F199" s="7"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E200" s="7"/>
+      <c r="F200" s="7"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E201" s="7"/>
+      <c r="F201" s="7"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E202" s="7"/>
+      <c r="F202" s="7"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E203" s="7"/>
+      <c r="F203" s="7"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E204" s="7"/>
+      <c r="F204" s="7"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E206" s="7"/>
+      <c r="F206" s="7"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E207" s="7"/>
+      <c r="F207" s="7"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E208" s="7"/>
+      <c r="F208" s="7"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E209" s="7"/>
+      <c r="F209" s="7"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E210" s="7"/>
+      <c r="F210" s="7"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E211" s="7"/>
+      <c r="F211" s="7"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E212" s="7"/>
+      <c r="F212" s="7"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E213" s="7"/>
+      <c r="F213" s="7"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E214" s="7"/>
+      <c r="F214" s="7"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E215" s="7"/>
+      <c r="F215" s="7"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E216" s="7"/>
+      <c r="F216" s="7"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E217" s="7"/>
+      <c r="F217" s="7"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E218" s="7"/>
+      <c r="F218" s="7"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E219" s="7"/>
+      <c r="F219" s="7"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E220" s="7"/>
+      <c r="F220" s="7"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E221" s="7"/>
+      <c r="F221" s="7"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E222" s="7"/>
+      <c r="F222" s="7"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E223" s="7"/>
+      <c r="F223" s="7"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E224" s="7"/>
+      <c r="F224" s="7"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E225" s="7"/>
+      <c r="F225" s="7"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E226" s="7"/>
+      <c r="F226" s="7"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E227" s="7"/>
+      <c r="F227" s="7"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E228" s="7"/>
+      <c r="F228" s="7"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E229" s="7"/>
+      <c r="F229" s="7"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E230" s="7"/>
+      <c r="F230" s="7"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E231" s="7"/>
+      <c r="F231" s="7"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E232" s="7"/>
+      <c r="F232" s="7"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E233" s="7"/>
+      <c r="F233" s="7"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E234" s="7"/>
+      <c r="F234" s="7"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E235" s="7"/>
+      <c r="F235" s="7"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E236" s="7"/>
+      <c r="F236" s="7"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E237" s="7"/>
+      <c r="F237" s="7"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E238" s="7"/>
+      <c r="F238" s="7"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E239" s="7"/>
+      <c r="F239" s="7"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E240" s="7"/>
+      <c r="F240" s="7"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E241" s="7"/>
+      <c r="F241" s="7"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E242" s="7"/>
+      <c r="F242" s="7"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E243" s="7"/>
+      <c r="F243" s="7"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E244" s="7"/>
+      <c r="F244" s="7"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E245" s="7"/>
+      <c r="F245" s="7"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E246" s="7"/>
+      <c r="F246" s="7"/>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E247" s="7"/>
+      <c r="F247" s="7"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E248" s="7"/>
+      <c r="F248" s="7"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E249" s="7"/>
+      <c r="F249" s="7"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E250" s="7"/>
+      <c r="F250" s="7"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E251" s="7"/>
+      <c r="F251" s="7"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E252" s="7"/>
+      <c r="F252" s="7"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E253" s="7"/>
+      <c r="F253" s="7"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E254" s="7"/>
+      <c r="F254" s="7"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E255" s="7"/>
+      <c r="F255" s="7"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E256" s="7"/>
+      <c r="F256" s="7"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E257" s="7"/>
+      <c r="F257" s="7"/>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E258" s="7"/>
+      <c r="F258" s="7"/>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E259" s="7"/>
+      <c r="F259" s="7"/>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E260" s="7"/>
+      <c r="F260" s="7"/>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E261" s="7"/>
+      <c r="F261" s="7"/>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E262" s="7"/>
+      <c r="F262" s="7"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E263" s="7"/>
+      <c r="F263" s="7"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E264" s="7"/>
+      <c r="F264" s="7"/>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E265" s="7"/>
+      <c r="F265" s="7"/>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E266" s="7"/>
+      <c r="F266" s="7"/>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E267" s="7"/>
+      <c r="F267" s="7"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E268" s="7"/>
+      <c r="F268" s="7"/>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E269" s="7"/>
+      <c r="F269" s="7"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E270" s="7"/>
+      <c r="F270" s="7"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E271" s="7"/>
+      <c r="F271" s="7"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E272" s="7"/>
+      <c r="F272" s="7"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E273" s="7"/>
+      <c r="F273" s="7"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E274" s="7"/>
+      <c r="F274" s="7"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E275" s="7"/>
+      <c r="F275" s="7"/>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E276" s="7"/>
+      <c r="F276" s="7"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E277" s="7"/>
+      <c r="F277" s="7"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E278" s="7"/>
+      <c r="F278" s="7"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E279" s="7"/>
+      <c r="F279" s="7"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E280" s="7"/>
+      <c r="F280" s="7"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E281" s="7"/>
+      <c r="F281" s="7"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E282" s="7"/>
+      <c r="F282" s="7"/>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E283" s="7"/>
+      <c r="F283" s="7"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E284" s="7"/>
+      <c r="F284" s="7"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E285" s="7"/>
+      <c r="F285" s="7"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E286" s="7"/>
+      <c r="F286" s="7"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E287" s="7"/>
+      <c r="F287" s="7"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E288" s="7"/>
+      <c r="F288" s="7"/>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E289" s="7"/>
+      <c r="F289" s="7"/>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E290" s="7"/>
+      <c r="F290" s="7"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E291" s="7"/>
+      <c r="F291" s="7"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E292" s="7"/>
+      <c r="F292" s="7"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E293" s="7"/>
+      <c r="F293" s="7"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E294" s="7"/>
+      <c r="F294" s="7"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E295" s="7"/>
+      <c r="F295" s="7"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E296" s="7"/>
+      <c r="F296" s="7"/>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E297" s="7"/>
+      <c r="F297" s="7"/>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E298" s="7"/>
+      <c r="F298" s="7"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E299" s="7"/>
+      <c r="F299" s="7"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E300" s="7"/>
+      <c r="F300" s="7"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E301" s="7"/>
+      <c r="F301" s="7"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E302" s="7"/>
+      <c r="F302" s="7"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E303" s="7"/>
+      <c r="F303" s="7"/>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E304" s="7"/>
+      <c r="F304" s="7"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E305" s="7"/>
+      <c r="F305" s="7"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E306" s="7"/>
+      <c r="F306" s="7"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E307" s="7"/>
+      <c r="F307" s="7"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E308" s="7"/>
+      <c r="F308" s="7"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E309" s="7"/>
+      <c r="F309" s="7"/>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E310" s="7"/>
+      <c r="F310" s="7"/>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E311" s="7"/>
+      <c r="F311" s="7"/>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E312" s="7"/>
+      <c r="F312" s="7"/>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E313" s="7"/>
+      <c r="F313" s="7"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E314" s="7"/>
+      <c r="F314" s="7"/>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E315" s="7"/>
+      <c r="F315" s="7"/>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E316" s="7"/>
+      <c r="F316" s="7"/>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E317" s="7"/>
+      <c r="F317" s="7"/>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E318" s="7"/>
+      <c r="F318" s="7"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E319" s="7"/>
+      <c r="F319" s="7"/>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E320" s="7"/>
+      <c r="F320" s="7"/>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E321" s="7"/>
+      <c r="F321" s="7"/>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E322" s="7"/>
+      <c r="F322" s="7"/>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E323" s="7"/>
+      <c r="F323" s="7"/>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E324" s="7"/>
+      <c r="F324" s="7"/>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E325" s="7"/>
+      <c r="F325" s="7"/>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E326" s="7"/>
+      <c r="F326" s="7"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E327" s="7"/>
+      <c r="F327" s="7"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E328" s="7"/>
+      <c r="F328" s="7"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E329" s="7"/>
+      <c r="F329" s="7"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E330" s="7"/>
+      <c r="F330" s="7"/>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E331" s="7"/>
+      <c r="F331" s="7"/>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E332" s="7"/>
+      <c r="F332" s="7"/>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E333" s="7"/>
+      <c r="F333" s="7"/>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E334" s="7"/>
+      <c r="F334" s="7"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E335" s="7"/>
+      <c r="F335" s="7"/>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E336" s="7"/>
+      <c r="F336" s="7"/>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E337" s="7"/>
+      <c r="F337" s="7"/>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E338" s="7"/>
+      <c r="F338" s="7"/>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E339" s="7"/>
+      <c r="F339" s="7"/>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E340" s="7"/>
+      <c r="F340" s="7"/>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E341" s="7"/>
+      <c r="F341" s="7"/>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E342" s="7"/>
+      <c r="F342" s="7"/>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E343" s="7"/>
+      <c r="F343" s="7"/>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E344" s="7"/>
+      <c r="F344" s="7"/>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E345" s="7"/>
+      <c r="F345" s="7"/>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E346" s="7"/>
+      <c r="F346" s="7"/>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E347" s="7"/>
+      <c r="F347" s="7"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E348" s="7"/>
+      <c r="F348" s="7"/>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E349" s="7"/>
+      <c r="F349" s="7"/>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E350" s="7"/>
+      <c r="F350" s="7"/>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E351" s="7"/>
+      <c r="F351" s="7"/>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E352" s="7"/>
+      <c r="F352" s="7"/>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E353" s="7"/>
+      <c r="F353" s="7"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E354" s="7"/>
+      <c r="F354" s="7"/>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E355" s="7"/>
+      <c r="F355" s="7"/>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E356" s="7"/>
+      <c r="F356" s="7"/>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E357" s="7"/>
+      <c r="F357" s="7"/>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E358" s="7"/>
+      <c r="F358" s="7"/>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E359" s="7"/>
+      <c r="F359" s="7"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E360" s="7"/>
+      <c r="F360" s="7"/>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E361" s="7"/>
+      <c r="F361" s="7"/>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E362" s="7"/>
+      <c r="F362" s="7"/>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E363" s="7"/>
+      <c r="F363" s="7"/>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E364" s="7"/>
+      <c r="F364" s="7"/>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E365" s="7"/>
+      <c r="F365" s="7"/>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E366" s="7"/>
+      <c r="F366" s="7"/>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E367" s="7"/>
+      <c r="F367" s="7"/>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E368" s="7"/>
+      <c r="F368" s="7"/>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E369" s="7"/>
+      <c r="F369" s="7"/>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E370" s="7"/>
+      <c r="F370" s="7"/>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E371" s="7"/>
+      <c r="F371" s="7"/>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E372" s="7"/>
+      <c r="F372" s="7"/>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E373" s="7"/>
+      <c r="F373" s="7"/>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E374" s="7"/>
+      <c r="F374" s="7"/>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E375" s="7"/>
+      <c r="F375" s="7"/>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E376" s="7"/>
+      <c r="F376" s="7"/>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E377" s="7"/>
+      <c r="F377" s="7"/>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E378" s="7"/>
+      <c r="F378" s="7"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E379" s="7"/>
+      <c r="F379" s="7"/>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E380" s="7"/>
+      <c r="F380" s="7"/>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E381" s="7"/>
+      <c r="F381" s="7"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E382" s="7"/>
+      <c r="F382" s="7"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E383" s="7"/>
+      <c r="F383" s="7"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E384" s="7"/>
+      <c r="F384" s="7"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E385" s="7"/>
+      <c r="F385" s="7"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E386" s="7"/>
+      <c r="F386" s="7"/>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E387" s="7"/>
+      <c r="F387" s="7"/>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E388" s="7"/>
+      <c r="F388" s="7"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E389" s="7"/>
+      <c r="F389" s="7"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E390" s="7"/>
+      <c r="F390" s="7"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E391" s="7"/>
+      <c r="F391" s="7"/>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E392" s="7"/>
+      <c r="F392" s="7"/>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E393" s="7"/>
+      <c r="F393" s="7"/>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E394" s="7"/>
+      <c r="F394" s="7"/>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E395" s="7"/>
+      <c r="F395" s="7"/>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E396" s="7"/>
+      <c r="F396" s="7"/>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E397" s="7"/>
+      <c r="F397" s="7"/>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E398" s="7"/>
+      <c r="F398" s="7"/>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E399" s="7"/>
+      <c r="F399" s="7"/>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E400" s="7"/>
+      <c r="F400" s="7"/>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E401" s="7"/>
+      <c r="F401" s="7"/>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E402" s="7"/>
+      <c r="F402" s="7"/>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E403" s="7"/>
+      <c r="F403" s="7"/>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E404" s="7"/>
+      <c r="F404" s="7"/>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E405" s="7"/>
+      <c r="F405" s="7"/>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E406" s="7"/>
+      <c r="F406" s="7"/>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E407" s="7"/>
+      <c r="F407" s="7"/>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E408" s="7"/>
+      <c r="F408" s="7"/>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E409" s="7"/>
+      <c r="F409" s="7"/>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E410" s="7"/>
+      <c r="F410" s="7"/>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E411" s="7"/>
+      <c r="F411" s="7"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E412" s="7"/>
+      <c r="F412" s="7"/>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E413" s="7"/>
+      <c r="F413" s="7"/>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E414" s="7"/>
+      <c r="F414" s="7"/>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E415" s="7"/>
+      <c r="F415" s="7"/>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E416" s="7"/>
+      <c r="F416" s="7"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E417" s="7"/>
+      <c r="F417" s="7"/>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E418" s="7"/>
+      <c r="F418" s="7"/>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E419" s="7"/>
+      <c r="F419" s="7"/>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E420" s="7"/>
+      <c r="F420" s="7"/>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E421" s="7"/>
+      <c r="F421" s="7"/>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E422" s="7"/>
+      <c r="F422" s="7"/>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E423" s="7"/>
+      <c r="F423" s="7"/>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E424" s="7"/>
+      <c r="F424" s="7"/>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E425" s="7"/>
+      <c r="F425" s="7"/>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E426" s="7"/>
+      <c r="F426" s="7"/>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E427" s="7"/>
+      <c r="F427" s="7"/>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E428" s="7"/>
+      <c r="F428" s="7"/>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E429" s="7"/>
+      <c r="F429" s="7"/>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E430" s="7"/>
+      <c r="F430" s="7"/>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E431" s="7"/>
+      <c r="F431" s="7"/>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E432" s="7"/>
+      <c r="F432" s="7"/>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E433" s="7"/>
+      <c r="F433" s="7"/>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E434" s="7"/>
+      <c r="F434" s="7"/>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E435" s="7"/>
+      <c r="F435" s="7"/>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E436" s="7"/>
+      <c r="F436" s="7"/>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E437" s="7"/>
+      <c r="F437" s="7"/>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E438" s="7"/>
+      <c r="F438" s="7"/>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E439" s="7"/>
+      <c r="F439" s="7"/>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E440" s="7"/>
+      <c r="F440" s="7"/>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E441" s="7"/>
+      <c r="F441" s="7"/>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E442" s="7"/>
+      <c r="F442" s="7"/>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E443" s="7"/>
+      <c r="F443" s="7"/>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E444" s="7"/>
+      <c r="F444" s="7"/>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E445" s="7"/>
+      <c r="F445" s="7"/>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E446" s="7"/>
+      <c r="F446" s="7"/>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E447" s="7"/>
+      <c r="F447" s="7"/>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E448" s="7"/>
+      <c r="F448" s="7"/>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E449" s="7"/>
+      <c r="F449" s="7"/>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E450" s="7"/>
+      <c r="F450" s="7"/>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E451" s="7"/>
+      <c r="F451" s="7"/>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E452" s="7"/>
+      <c r="F452" s="7"/>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E453" s="7"/>
+      <c r="F453" s="7"/>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E454" s="7"/>
+      <c r="F454" s="7"/>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E455" s="7"/>
+      <c r="F455" s="7"/>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E456" s="7"/>
+      <c r="F456" s="7"/>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E457" s="7"/>
+      <c r="F457" s="7"/>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E458" s="7"/>
+      <c r="F458" s="7"/>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E459" s="7"/>
+      <c r="F459" s="7"/>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E460" s="7"/>
+      <c r="F460" s="7"/>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E461" s="7"/>
+      <c r="F461" s="7"/>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E462" s="7"/>
+      <c r="F462" s="7"/>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E463" s="7"/>
+      <c r="F463" s="7"/>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E464" s="7"/>
+      <c r="F464" s="7"/>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E465" s="7"/>
+      <c r="F465" s="7"/>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E466" s="7"/>
+      <c r="F466" s="7"/>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E467" s="7"/>
+      <c r="F467" s="7"/>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E468" s="7"/>
+      <c r="F468" s="7"/>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E469" s="7"/>
+      <c r="F469" s="7"/>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E470" s="7"/>
+      <c r="F470" s="7"/>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E471" s="7"/>
+      <c r="F471" s="7"/>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E472" s="7"/>
+      <c r="F472" s="7"/>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E473" s="7"/>
+      <c r="F473" s="7"/>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E474" s="7"/>
+      <c r="F474" s="7"/>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E475" s="7"/>
+      <c r="F475" s="7"/>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E476" s="7"/>
+      <c r="F476" s="7"/>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E477" s="7"/>
+      <c r="F477" s="7"/>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E478" s="7"/>
+      <c r="F478" s="7"/>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E479" s="7"/>
+      <c r="F479" s="7"/>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E480" s="7"/>
+      <c r="F480" s="7"/>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E481" s="7"/>
+      <c r="F481" s="7"/>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E482" s="7"/>
+      <c r="F482" s="7"/>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E483" s="7"/>
+      <c r="F483" s="7"/>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E484" s="7"/>
+      <c r="F484" s="7"/>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E485" s="7"/>
+      <c r="F485" s="7"/>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E486" s="7"/>
+      <c r="F486" s="7"/>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E487" s="7"/>
+      <c r="F487" s="7"/>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E488" s="7"/>
+      <c r="F488" s="7"/>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E489" s="7"/>
+      <c r="F489" s="7"/>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E490" s="7"/>
+      <c r="F490" s="7"/>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E491" s="7"/>
+      <c r="F491" s="7"/>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E492" s="7"/>
+      <c r="F492" s="7"/>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E493" s="7"/>
+      <c r="F493" s="7"/>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E494" s="7"/>
+      <c r="F494" s="7"/>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E495" s="7"/>
+      <c r="F495" s="7"/>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E496" s="7"/>
+      <c r="F496" s="7"/>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E497" s="7"/>
+      <c r="F497" s="7"/>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E498" s="7"/>
+      <c r="F498" s="7"/>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E499" s="7"/>
+      <c r="F499" s="7"/>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E500" s="7"/>
+      <c r="F500" s="7"/>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E501" s="7"/>
+      <c r="F501" s="7"/>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E502" s="7"/>
+      <c r="F502" s="7"/>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E503" s="7"/>
+      <c r="F503" s="7"/>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E504" s="7"/>
+      <c r="F504" s="7"/>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E505" s="7"/>
+      <c r="F505" s="7"/>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E506" s="7"/>
+      <c r="F506" s="7"/>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E507" s="7"/>
+      <c r="F507" s="7"/>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E508" s="7"/>
+      <c r="F508" s="7"/>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E509" s="7"/>
+      <c r="F509" s="7"/>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E510" s="7"/>
+      <c r="F510" s="7"/>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E511" s="7"/>
+      <c r="F511" s="7"/>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E512" s="7"/>
+      <c r="F512" s="7"/>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E513" s="7"/>
+      <c r="F513" s="7"/>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E514" s="7"/>
+      <c r="F514" s="7"/>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E515" s="7"/>
+      <c r="F515" s="7"/>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E516" s="7"/>
+      <c r="F516" s="7"/>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E517" s="7"/>
+      <c r="F517" s="7"/>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E518" s="7"/>
+      <c r="F518" s="7"/>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E519" s="7"/>
+      <c r="F519" s="7"/>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E520" s="7"/>
+      <c r="F520" s="7"/>
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E521" s="7"/>
+      <c r="F521" s="7"/>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E522" s="7"/>
+      <c r="F522" s="7"/>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E523" s="7"/>
+      <c r="F523" s="7"/>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E524" s="7"/>
+      <c r="F524" s="7"/>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E525" s="7"/>
+      <c r="F525" s="7"/>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E526" s="7"/>
+      <c r="F526" s="7"/>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E527" s="7"/>
+      <c r="F527" s="7"/>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E528" s="7"/>
+      <c r="F528" s="7"/>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E529" s="7"/>
+      <c r="F529" s="7"/>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E530" s="7"/>
+      <c r="F530" s="7"/>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E531" s="7"/>
+      <c r="F531" s="7"/>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E532" s="7"/>
+      <c r="F532" s="7"/>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E533" s="7"/>
+      <c r="F533" s="7"/>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E534" s="7"/>
+      <c r="F534" s="7"/>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E535" s="7"/>
+      <c r="F535" s="7"/>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E536" s="7"/>
+      <c r="F536" s="7"/>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E537" s="7"/>
+      <c r="F537" s="7"/>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E538" s="7"/>
+      <c r="F538" s="7"/>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E539" s="7"/>
+      <c r="F539" s="7"/>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E540" s="7"/>
+      <c r="F540" s="7"/>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E541" s="7"/>
+      <c r="F541" s="7"/>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E542" s="7"/>
+      <c r="F542" s="7"/>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E543" s="7"/>
+      <c r="F543" s="7"/>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E544" s="7"/>
+      <c r="F544" s="7"/>
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E545" s="7"/>
+      <c r="F545" s="7"/>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E546" s="7"/>
+      <c r="F546" s="7"/>
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E547" s="7"/>
+      <c r="F547" s="7"/>
     </row>
     <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E548" s="7"/>
+      <c r="F548" s="7"/>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E549" s="7"/>
+      <c r="F549" s="7"/>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E550" s="7"/>
+      <c r="F550" s="7"/>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E551" s="7"/>
+      <c r="F551" s="7"/>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E552" s="7"/>
+      <c r="F552" s="7"/>
     </row>
     <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E553" s="7"/>
+      <c r="F553" s="7"/>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E554" s="7"/>
+      <c r="F554" s="7"/>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E555" s="7"/>
+      <c r="F555" s="7"/>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E556" s="7"/>
+      <c r="F556" s="7"/>
     </row>
     <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E557" s="7"/>
+      <c r="F557" s="7"/>
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E558" s="7"/>
+      <c r="F558" s="7"/>
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E559" s="7"/>
+      <c r="F559" s="7"/>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E560" s="7"/>
+      <c r="F560" s="7"/>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E561" s="7"/>
+      <c r="F561" s="7"/>
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E562" s="7"/>
+      <c r="F562" s="7"/>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E563" s="7"/>
+      <c r="F563" s="7"/>
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E564" s="7"/>
+      <c r="F564" s="7"/>
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E565" s="7"/>
+      <c r="F565" s="7"/>
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E566" s="7"/>
+      <c r="F566" s="7"/>
     </row>
     <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E567" s="7"/>
+      <c r="F567" s="7"/>
     </row>
     <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E568" s="7"/>
+      <c r="F568" s="7"/>
     </row>
     <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E569" s="7"/>
+      <c r="F569" s="7"/>
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E570" s="7"/>
+      <c r="F570" s="7"/>
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E571" s="7"/>
+      <c r="F571" s="7"/>
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E572" s="7"/>
+      <c r="F572" s="7"/>
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E573" s="7"/>
+      <c r="F573" s="7"/>
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E574" s="7"/>
+      <c r="F574" s="7"/>
     </row>
     <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E575" s="7"/>
+      <c r="F575" s="7"/>
     </row>
     <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E576" s="7"/>
+      <c r="F576" s="7"/>
     </row>
     <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E577" s="7"/>
+      <c r="F577" s="7"/>
     </row>
     <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E578" s="7"/>
+      <c r="F578" s="7"/>
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E579" s="7"/>
+      <c r="F579" s="7"/>
     </row>
     <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E580" s="7"/>
+      <c r="F580" s="7"/>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E581" s="7"/>
+      <c r="F581" s="7"/>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E582" s="7"/>
+      <c r="F582" s="7"/>
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E583" s="7"/>
+      <c r="F583" s="7"/>
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E584" s="7"/>
+      <c r="F584" s="7"/>
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E585" s="7"/>
+      <c r="F585" s="7"/>
     </row>
     <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E586" s="7"/>
+      <c r="F586" s="7"/>
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E587" s="7"/>
+      <c r="F587" s="7"/>
     </row>
     <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E588" s="7"/>
+      <c r="F588" s="7"/>
     </row>
     <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E589" s="7"/>
+      <c r="F589" s="7"/>
     </row>
     <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E590" s="7"/>
+      <c r="F590" s="7"/>
     </row>
     <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E591" s="7"/>
+      <c r="F591" s="7"/>
     </row>
     <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E592" s="7"/>
+      <c r="F592" s="7"/>
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E593" s="7"/>
+      <c r="F593" s="7"/>
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E594" s="7"/>
+      <c r="F594" s="7"/>
     </row>
     <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E595" s="7"/>
+      <c r="F595" s="7"/>
     </row>
     <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E596" s="7"/>
+      <c r="F596" s="7"/>
     </row>
     <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E597" s="7"/>
+      <c r="F597" s="7"/>
     </row>
     <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E598" s="7"/>
+      <c r="F598" s="7"/>
     </row>
     <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E599" s="7"/>
+      <c r="F599" s="7"/>
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E600" s="7"/>
+      <c r="F600" s="7"/>
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E601" s="7"/>
+      <c r="F601" s="7"/>
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E602" s="7"/>
+      <c r="F602" s="7"/>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E603" s="7"/>
+      <c r="F603" s="7"/>
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E604" s="7"/>
+      <c r="F604" s="7"/>
     </row>
     <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E605" s="7"/>
+      <c r="F605" s="7"/>
     </row>
     <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E606" s="7"/>
+      <c r="F606" s="7"/>
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E607" s="7"/>
+      <c r="F607" s="7"/>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E608" s="7"/>
+      <c r="F608" s="7"/>
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E609" s="7"/>
+      <c r="F609" s="7"/>
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E610" s="7"/>
+      <c r="F610" s="7"/>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E611" s="7"/>
+      <c r="F611" s="7"/>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E612" s="7"/>
+      <c r="F612" s="7"/>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E613" s="7"/>
+      <c r="F613" s="7"/>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E614" s="7"/>
+      <c r="F614" s="7"/>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E615" s="7"/>
+      <c r="F615" s="7"/>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E616" s="7"/>
+      <c r="F616" s="7"/>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E617" s="7"/>
+      <c r="F617" s="7"/>
     </row>
     <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E618" s="7"/>
+      <c r="F618" s="7"/>
     </row>
     <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E619" s="7"/>
+      <c r="F619" s="7"/>
     </row>
     <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E620" s="7"/>
+      <c r="F620" s="7"/>
     </row>
     <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E621" s="7"/>
+      <c r="F621" s="7"/>
     </row>
     <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E622" s="7"/>
+      <c r="F622" s="7"/>
     </row>
     <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E623" s="7"/>
+      <c r="F623" s="7"/>
     </row>
     <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E624" s="7"/>
+      <c r="F624" s="7"/>
     </row>
     <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E625" s="7"/>
+      <c r="F625" s="7"/>
     </row>
     <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E626" s="7"/>
+      <c r="F626" s="7"/>
     </row>
     <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E627" s="7"/>
+      <c r="F627" s="7"/>
     </row>
     <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E628" s="7"/>
+      <c r="F628" s="7"/>
     </row>
     <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E629" s="7"/>
+      <c r="F629" s="7"/>
     </row>
     <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E630" s="7"/>
+      <c r="F630" s="7"/>
     </row>
     <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E631" s="7"/>
+      <c r="F631" s="7"/>
     </row>
     <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E632" s="7"/>
+      <c r="F632" s="7"/>
     </row>
     <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E633" s="7"/>
+      <c r="F633" s="7"/>
     </row>
     <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E634" s="7"/>
+      <c r="F634" s="7"/>
     </row>
     <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E635" s="7"/>
+      <c r="F635" s="7"/>
     </row>
     <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E636" s="7"/>
+      <c r="F636" s="7"/>
     </row>
     <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E637" s="7"/>
+      <c r="F637" s="7"/>
     </row>
     <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E638" s="7"/>
+      <c r="F638" s="7"/>
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E639" s="7"/>
+      <c r="F639" s="7"/>
     </row>
     <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E640" s="7"/>
+      <c r="F640" s="7"/>
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E641" s="7"/>
+      <c r="F641" s="7"/>
     </row>
     <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E642" s="7"/>
+      <c r="F642" s="7"/>
     </row>
     <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E643" s="7"/>
+      <c r="F643" s="7"/>
     </row>
     <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E644" s="7"/>
+      <c r="F644" s="7"/>
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E645" s="7"/>
+      <c r="F645" s="7"/>
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E646" s="7"/>
+      <c r="F646" s="7"/>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E647" s="7"/>
+      <c r="F647" s="7"/>
     </row>
     <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E648" s="7"/>
+      <c r="F648" s="7"/>
     </row>
     <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E649" s="7"/>
+      <c r="F649" s="7"/>
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E650" s="7"/>
+      <c r="F650" s="7"/>
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E651" s="7"/>
+      <c r="F651" s="7"/>
     </row>
     <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E652" s="7"/>
+      <c r="F652" s="7"/>
     </row>
     <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E653" s="7"/>
+      <c r="F653" s="7"/>
     </row>
     <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E654" s="7"/>
+      <c r="F654" s="7"/>
     </row>
     <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E655" s="7"/>
+      <c r="F655" s="7"/>
     </row>
     <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E656" s="7"/>
+      <c r="F656" s="7"/>
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E657" s="7"/>
+      <c r="F657" s="7"/>
     </row>
     <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E658" s="7"/>
+      <c r="F658" s="7"/>
     </row>
     <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E659" s="7"/>
+      <c r="F659" s="7"/>
     </row>
     <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E660" s="7"/>
+      <c r="F660" s="7"/>
     </row>
     <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E661" s="7"/>
+      <c r="F661" s="7"/>
     </row>
     <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E662" s="7"/>
+      <c r="F662" s="7"/>
     </row>
     <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E663" s="7"/>
+      <c r="F663" s="7"/>
     </row>
     <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E664" s="7"/>
+      <c r="F664" s="7"/>
     </row>
     <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E665" s="7"/>
+      <c r="F665" s="7"/>
     </row>
     <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E666" s="7"/>
+      <c r="F666" s="7"/>
     </row>
     <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E667" s="7"/>
+      <c r="F667" s="7"/>
     </row>
     <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E668" s="7"/>
+      <c r="F668" s="7"/>
     </row>
     <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E669" s="7"/>
+      <c r="F669" s="7"/>
     </row>
     <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E670" s="7"/>
+      <c r="F670" s="7"/>
     </row>
     <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E671" s="7"/>
+      <c r="F671" s="7"/>
     </row>
     <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E672" s="7"/>
+      <c r="F672" s="7"/>
     </row>
     <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E673" s="7"/>
+      <c r="F673" s="7"/>
     </row>
     <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E674" s="7"/>
+      <c r="F674" s="7"/>
     </row>
     <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E675" s="7"/>
+      <c r="F675" s="7"/>
     </row>
     <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E676" s="7"/>
+      <c r="F676" s="7"/>
     </row>
     <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E677" s="7"/>
+      <c r="F677" s="7"/>
     </row>
     <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E678" s="7"/>
+      <c r="F678" s="7"/>
     </row>
     <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E679" s="7"/>
+      <c r="F679" s="7"/>
     </row>
     <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E680" s="7"/>
+      <c r="F680" s="7"/>
     </row>
     <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E681" s="7"/>
+      <c r="F681" s="7"/>
     </row>
     <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E682" s="7"/>
+      <c r="F682" s="7"/>
     </row>
     <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E683" s="7"/>
+      <c r="F683" s="7"/>
     </row>
     <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E684" s="7"/>
+      <c r="F684" s="7"/>
     </row>
     <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E685" s="7"/>
+      <c r="F685" s="7"/>
     </row>
     <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E686" s="7"/>
+      <c r="F686" s="7"/>
     </row>
     <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E687" s="7"/>
+      <c r="F687" s="7"/>
     </row>
     <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E688" s="7"/>
+      <c r="F688" s="7"/>
     </row>
     <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E689" s="7"/>
+      <c r="F689" s="7"/>
     </row>
     <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E690" s="7"/>
+      <c r="F690" s="7"/>
     </row>
     <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E691" s="7"/>
+      <c r="F691" s="7"/>
     </row>
     <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E692" s="7"/>
+      <c r="F692" s="7"/>
     </row>
     <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E693" s="7"/>
+      <c r="F693" s="7"/>
     </row>
     <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E694" s="7"/>
+      <c r="F694" s="7"/>
     </row>
     <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E695" s="7"/>
+      <c r="F695" s="7"/>
     </row>
     <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E696" s="7"/>
+      <c r="F696" s="7"/>
     </row>
     <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E697" s="7"/>
+      <c r="F697" s="7"/>
     </row>
     <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E698" s="7"/>
+      <c r="F698" s="7"/>
     </row>
     <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E699" s="7"/>
+      <c r="F699" s="7"/>
     </row>
     <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E700" s="7"/>
+      <c r="F700" s="7"/>
     </row>
     <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E701" s="7"/>
+      <c r="F701" s="7"/>
     </row>
     <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E702" s="7"/>
+      <c r="F702" s="7"/>
     </row>
     <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E703" s="7"/>
+      <c r="F703" s="7"/>
     </row>
     <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E704" s="7"/>
+      <c r="F704" s="7"/>
     </row>
     <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E705" s="7"/>
+      <c r="F705" s="7"/>
     </row>
     <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E706" s="7"/>
+      <c r="F706" s="7"/>
     </row>
     <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E707" s="7"/>
+      <c r="F707" s="7"/>
     </row>
     <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E708" s="7"/>
+      <c r="F708" s="7"/>
     </row>
     <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E709" s="7"/>
+      <c r="F709" s="7"/>
     </row>
     <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E710" s="7"/>
+      <c r="F710" s="7"/>
     </row>
     <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E711" s="7"/>
+      <c r="F711" s="7"/>
     </row>
     <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E712" s="7"/>
+      <c r="F712" s="7"/>
     </row>
     <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E713" s="7"/>
+      <c r="F713" s="7"/>
     </row>
     <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E714" s="7"/>
+      <c r="F714" s="7"/>
     </row>
     <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E715" s="7"/>
+      <c r="F715" s="7"/>
     </row>
     <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E716" s="7"/>
+      <c r="F716" s="7"/>
     </row>
     <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E717" s="7"/>
+      <c r="F717" s="7"/>
     </row>
     <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E718" s="7"/>
+      <c r="F718" s="7"/>
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E719" s="7"/>
+      <c r="F719" s="7"/>
     </row>
     <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E720" s="7"/>
+      <c r="F720" s="7"/>
     </row>
     <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E721" s="7"/>
+      <c r="F721" s="7"/>
     </row>
     <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E722" s="7"/>
+      <c r="F722" s="7"/>
     </row>
     <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E723" s="7"/>
+      <c r="F723" s="7"/>
     </row>
     <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E724" s="7"/>
+      <c r="F724" s="7"/>
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E725" s="7"/>
+      <c r="F725" s="7"/>
     </row>
     <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E726" s="7"/>
+      <c r="F726" s="7"/>
     </row>
     <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E727" s="7"/>
+      <c r="F727" s="7"/>
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E728" s="7"/>
+      <c r="F728" s="7"/>
     </row>
     <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E729" s="7"/>
+      <c r="F729" s="7"/>
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E730" s="7"/>
+      <c r="F730" s="7"/>
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E731" s="7"/>
+      <c r="F731" s="7"/>
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E732" s="7"/>
+      <c r="F732" s="7"/>
     </row>
     <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E733" s="7"/>
+      <c r="F733" s="7"/>
     </row>
     <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E734" s="7"/>
+      <c r="F734" s="7"/>
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E735" s="7"/>
+      <c r="F735" s="7"/>
     </row>
     <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E736" s="7"/>
+      <c r="F736" s="7"/>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E737" s="7"/>
+      <c r="F737" s="7"/>
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E738" s="7"/>
+      <c r="F738" s="7"/>
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E739" s="7"/>
+      <c r="F739" s="7"/>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E740" s="7"/>
+      <c r="F740" s="7"/>
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E741" s="7"/>
+      <c r="F741" s="7"/>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E742" s="7"/>
+      <c r="F742" s="7"/>
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E743" s="7"/>
+      <c r="F743" s="7"/>
     </row>
     <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E744" s="7"/>
+      <c r="F744" s="7"/>
     </row>
     <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E745" s="7"/>
+      <c r="F745" s="7"/>
     </row>
     <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E746" s="7"/>
+      <c r="F746" s="7"/>
     </row>
     <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E747" s="7"/>
+      <c r="F747" s="7"/>
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E748" s="7"/>
+      <c r="F748" s="7"/>
     </row>
     <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E749" s="7"/>
+      <c r="F749" s="7"/>
     </row>
     <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E750" s="7"/>
+      <c r="F750" s="7"/>
     </row>
     <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E751" s="7"/>
+      <c r="F751" s="7"/>
     </row>
     <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E752" s="7"/>
+      <c r="F752" s="7"/>
     </row>
     <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E753" s="7"/>
+      <c r="F753" s="7"/>
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E754" s="7"/>
+      <c r="F754" s="7"/>
     </row>
     <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E755" s="7"/>
+      <c r="F755" s="7"/>
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E756" s="7"/>
+      <c r="F756" s="7"/>
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E757" s="7"/>
+      <c r="F757" s="7"/>
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E758" s="7"/>
+      <c r="F758" s="7"/>
     </row>
     <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E759" s="7"/>
+      <c r="F759" s="7"/>
     </row>
     <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E760" s="7"/>
+      <c r="F760" s="7"/>
     </row>
     <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E761" s="7"/>
+      <c r="F761" s="7"/>
     </row>
     <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E762" s="7"/>
+      <c r="F762" s="7"/>
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E763" s="7"/>
+      <c r="F763" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -11989,11 +12125,11 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.90625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.94921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.01"/>
@@ -12006,41 +12142,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20210221001</v>
@@ -12048,29 +12184,29 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -12078,49 +12214,49 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Update new member forms
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="547">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1391,9 +1391,6 @@
     <t xml:space="preserve">member_emigrated_when_date</t>
   </si>
   <si>
-    <t xml:space="preserve">member_emigrated_when_num</t>
-  </si>
-  <si>
     <t xml:space="preserve">member_emigrated_when_dmy_ago</t>
   </si>
   <si>
@@ -1407,9 +1404,6 @@
   </si>
   <si>
     <t xml:space="preserve">new_member_move_in_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_member_move_in_enter</t>
   </si>
   <si>
     <t xml:space="preserve">new_member_move_in_select</t>
@@ -1983,7 +1977,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -3028,7 +3022,7 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13"/>
@@ -4404,7 +4398,7 @@
       <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -8860,13 +8854,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H760"/>
+  <dimension ref="A1:H758"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -9271,9 +9265,12 @@
         <v>455</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>429</v>
+        <v>33</v>
       </c>
       <c r="D33" s="11"/>
+      <c r="E33" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="F33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9285,37 +9282,34 @@
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="0" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="F34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="B35" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="11"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="0" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="F35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>458</v>
-      </c>
       <c r="B36" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>33</v>
+        <v>452</v>
       </c>
       <c r="D36" s="12"/>
-      <c r="E36" s="0" t="s">
-        <v>188</v>
-      </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9323,9 +9317,12 @@
         <v>460</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>452</v>
+        <v>33</v>
       </c>
       <c r="D37" s="12"/>
+      <c r="E37" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9333,9 +9330,12 @@
         <v>461</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>429</v>
+        <v>33</v>
       </c>
       <c r="D38" s="12"/>
+      <c r="E38" s="0" t="s">
+        <v>137</v>
+      </c>
       <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9347,7 +9347,7 @@
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="0" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="F39" s="7"/>
     </row>
@@ -9356,35 +9356,38 @@
         <v>463</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="0" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="F40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="B41" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="C42" s="12" t="s">
+      <c r="B42" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="D42" s="12"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="0" t="s">
         <v>40</v>
       </c>
@@ -9392,44 +9395,41 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="B43" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="0" t="s">
-        <v>44</v>
-      </c>
+      <c r="B43" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="D43" s="13"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="9" t="s">
-        <v>468</v>
-      </c>
-      <c r="C44" s="9" t="s">
+      <c r="B44" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>441</v>
       </c>
-      <c r="D44" s="9"/>
+      <c r="D44" s="13"/>
       <c r="E44" s="0" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="F44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>469</v>
-      </c>
       <c r="B45" s="13" t="s">
         <v>470</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>429</v>
+        <v>33</v>
       </c>
       <c r="D45" s="13"/>
+      <c r="E45" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="F45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9437,12 +9437,9 @@
         <v>471</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="D46" s="13"/>
-      <c r="E46" s="0" t="s">
-        <v>175</v>
-      </c>
       <c r="F46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9450,11 +9447,11 @@
         <v>472</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F47" s="7"/>
     </row>
@@ -9463,9 +9460,12 @@
         <v>473</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="D48" s="13"/>
+      <c r="E48" s="0" t="s">
+        <v>78</v>
+      </c>
       <c r="F48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9473,12 +9473,9 @@
         <v>474</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D49" s="13"/>
-      <c r="E49" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="F49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9486,41 +9483,44 @@
         <v>475</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="13" t="s">
+      <c r="A51" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>437</v>
-      </c>
-      <c r="D51" s="13"/>
+      <c r="B51" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="F51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="13" t="s">
-        <v>477</v>
-      </c>
-      <c r="C52" s="13" t="s">
+      <c r="B52" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D52" s="13"/>
+      <c r="D52" s="14"/>
       <c r="E52" s="0" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="F52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>478</v>
-      </c>
       <c r="B53" s="14" t="s">
         <v>479</v>
       </c>
@@ -9538,12 +9538,9 @@
         <v>480</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D54" s="14"/>
-      <c r="E54" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="F54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9574,12 +9571,9 @@
         <v>483</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D57" s="14"/>
-      <c r="E57" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="F57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9587,9 +9581,12 @@
         <v>484</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D58" s="14"/>
+      <c r="E58" s="0" t="s">
+        <v>204</v>
+      </c>
       <c r="F58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9597,60 +9594,63 @@
         <v>485</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D59" s="14"/>
+      <c r="E59" s="0" t="s">
+        <v>209</v>
+      </c>
       <c r="F59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="14" t="s">
-        <v>486</v>
+        <v>140</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="0" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="F60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="C61" s="14" t="s">
         <v>487</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="0" t="s">
-        <v>209</v>
+        <v>488</v>
       </c>
       <c r="F61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="14" t="s">
-        <v>140</v>
+        <v>489</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="0" t="s">
-        <v>140</v>
+        <v>252</v>
       </c>
       <c r="F62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="14" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>489</v>
+        <v>441</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="0" t="s">
-        <v>490</v>
+        <v>92</v>
       </c>
       <c r="F63" s="7"/>
     </row>
@@ -9659,12 +9659,9 @@
         <v>491</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D64" s="14"/>
-      <c r="E64" s="0" t="s">
-        <v>252</v>
-      </c>
       <c r="F64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9672,11 +9669,11 @@
         <v>492</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="0" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="F65" s="7"/>
     </row>
@@ -9685,9 +9682,12 @@
         <v>493</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D66" s="14"/>
+      <c r="E66" s="0" t="s">
+        <v>191</v>
+      </c>
       <c r="F66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9695,12 +9695,9 @@
         <v>494</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>33</v>
+        <v>437</v>
       </c>
       <c r="D67" s="14"/>
-      <c r="E67" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="F67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9712,7 +9709,7 @@
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="0" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F68" s="7"/>
     </row>
@@ -9731,11 +9728,11 @@
         <v>497</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D70" s="14"/>
       <c r="E70" s="0" t="s">
-        <v>196</v>
+        <v>41</v>
       </c>
       <c r="F70" s="7"/>
     </row>
@@ -9744,9 +9741,12 @@
         <v>498</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D71" s="14"/>
+      <c r="E71" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="F71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9754,12 +9754,9 @@
         <v>499</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>33</v>
+        <v>437</v>
       </c>
       <c r="D72" s="14"/>
-      <c r="E72" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="F72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9767,11 +9764,11 @@
         <v>500</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="0" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F73" s="7"/>
     </row>
@@ -9780,9 +9777,12 @@
         <v>501</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>437</v>
+        <v>33</v>
       </c>
       <c r="D74" s="14"/>
+      <c r="E74" s="0" t="s">
+        <v>168</v>
+      </c>
       <c r="F74" s="7"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="D76" s="14"/>
       <c r="E76" s="0" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F76" s="7"/>
     </row>
@@ -9816,11 +9816,11 @@
         <v>504</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="0" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="F77" s="7"/>
     </row>
@@ -9829,11 +9829,11 @@
         <v>505</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="0" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F78" s="7"/>
     </row>
@@ -9842,11 +9842,11 @@
         <v>506</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="0" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="F79" s="7"/>
     </row>
@@ -9855,11 +9855,11 @@
         <v>507</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D80" s="14"/>
       <c r="E80" s="0" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="F80" s="7"/>
     </row>
@@ -9885,7 +9885,7 @@
       </c>
       <c r="D82" s="14"/>
       <c r="E82" s="0" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="F82" s="7"/>
     </row>
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D83" s="14"/>
       <c r="E83" s="0" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F83" s="7"/>
     </row>
@@ -9911,7 +9911,7 @@
       </c>
       <c r="D84" s="14"/>
       <c r="E84" s="0" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="F84" s="7"/>
     </row>
@@ -9924,7 +9924,7 @@
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="0" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="F85" s="7"/>
     </row>
@@ -9937,7 +9937,7 @@
       </c>
       <c r="D86" s="14"/>
       <c r="E86" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F86" s="7"/>
     </row>
@@ -9946,12 +9946,9 @@
         <v>514</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>33</v>
+        <v>429</v>
       </c>
       <c r="D87" s="14"/>
-      <c r="E87" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="F87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9963,43 +9960,46 @@
       </c>
       <c r="D88" s="14"/>
       <c r="E88" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="14" t="s">
-        <v>516</v>
+        <v>239</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>429</v>
+        <v>33</v>
       </c>
       <c r="D89" s="14"/>
+      <c r="E89" s="0" t="s">
+        <v>239</v>
+      </c>
       <c r="F89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="0" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="F90" s="7"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
-        <v>239</v>
+        <v>517</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D91" s="14"/>
       <c r="E91" s="0" t="s">
-        <v>239</v>
+        <v>60</v>
       </c>
       <c r="F91" s="7"/>
     </row>
@@ -10012,7 +10012,7 @@
       </c>
       <c r="D92" s="14"/>
       <c r="E92" s="0" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F92" s="7"/>
     </row>
@@ -10021,11 +10021,11 @@
         <v>519</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="D93" s="14"/>
       <c r="E93" s="0" t="s">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="F93" s="7"/>
     </row>
@@ -10034,11 +10034,11 @@
         <v>520</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>33</v>
+        <v>441</v>
       </c>
       <c r="D94" s="14"/>
       <c r="E94" s="0" t="s">
-        <v>228</v>
+        <v>72</v>
       </c>
       <c r="F94" s="7"/>
     </row>
@@ -10051,70 +10051,50 @@
       </c>
       <c r="D95" s="14"/>
       <c r="E95" s="0" t="s">
-        <v>240</v>
+        <v>41</v>
       </c>
       <c r="F95" s="7"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="14" t="s">
-        <v>522</v>
+        <v>241</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>441</v>
       </c>
       <c r="D96" s="14"/>
       <c r="E96" s="0" t="s">
-        <v>72</v>
+        <v>241</v>
       </c>
       <c r="F96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="14"/>
       <c r="E97" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F97" s="7"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="14" t="s">
-        <v>241</v>
+        <v>523</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="D98" s="14"/>
-      <c r="E98" s="0" t="s">
-        <v>241</v>
-      </c>
       <c r="F98" s="7"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="14" t="s">
-        <v>524</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D99" s="14"/>
-      <c r="E99" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F99" s="7"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="14" t="s">
-        <v>525</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>429</v>
-      </c>
-      <c r="D100" s="14"/>
       <c r="F100" s="7"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12090,12 +12070,6 @@
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F758" s="7"/>
-    </row>
-    <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F759" s="7"/>
-    </row>
-    <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F760" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -12115,11 +12089,11 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.01"/>
@@ -12132,71 +12106,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>526</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>527</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>528</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>529</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>530</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>531</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210224001</v>
+        <v>20210225001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -12204,49 +12178,49 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Implement change requests from Imani
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member_absent/hh_member_absent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="549">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1313,10 +1313,13 @@
     <t xml:space="preserve">extIdObj</t>
   </si>
   <si>
+    <t xml:space="preserve">override_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
     <t xml:space="preserve">form_status_hh_member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
   </si>
   <si>
     <t xml:space="preserve">form_status_hh_member_absent</t>
@@ -1980,7 +1983,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.08203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.09765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -3025,7 +3028,7 @@
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.09765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13"/>
@@ -4412,7 +4415,7 @@
       <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -8868,13 +8871,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H758"/>
+  <dimension ref="A1:H759"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -8973,7 +8976,9 @@
         <v>430</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
@@ -9036,24 +9041,24 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B13" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>439</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>438</v>
       </c>
       <c r="D14" s="9"/>
       <c r="F14" s="7"/>
@@ -9063,7 +9068,7 @@
         <v>440</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="D15" s="9"/>
       <c r="F15" s="7"/>
@@ -9073,22 +9078,22 @@
         <v>441</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>430</v>
-      </c>
       <c r="D17" s="9"/>
+      <c r="E17" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9096,12 +9101,9 @@
         <v>444</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9109,9 +9111,12 @@
         <v>445</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="D19" s="9"/>
+      <c r="E19" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9119,12 +9124,9 @@
         <v>446</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9132,9 +9134,12 @@
         <v>447</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="D21" s="9"/>
+      <c r="E21" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9142,126 +9147,123 @@
         <v>448</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="F22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
-        <v>135</v>
+        <v>449</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="0" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="F23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="0" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
       <c r="F24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
-        <v>449</v>
+        <v>224</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>438</v>
+        <v>34</v>
       </c>
       <c r="D25" s="9"/>
+      <c r="E25" s="0" t="s">
+        <v>224</v>
+      </c>
       <c r="F25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="B26" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="0" t="s">
+      <c r="D27" s="10"/>
+      <c r="E27" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="10"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="0" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>451</v>
-      </c>
-      <c r="B29" s="11" t="s">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="0" t="s">
+      <c r="D30" s="11"/>
+      <c r="E30" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="D30" s="11"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>442</v>
-      </c>
       <c r="D31" s="11"/>
-      <c r="E31" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9269,9 +9271,12 @@
         <v>455</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="D32" s="11"/>
+      <c r="E32" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="F32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9279,12 +9284,9 @@
         <v>456</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="D33" s="11"/>
-      <c r="E33" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9292,38 +9294,41 @@
         <v>457</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="B35" s="12" t="s">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>459</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="12" t="s">
         <v>460</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>453</v>
+        <v>34</v>
       </c>
       <c r="D36" s="12"/>
+      <c r="E36" s="0" t="s">
+        <v>189</v>
+      </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9331,12 +9336,9 @@
         <v>461</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="D37" s="12"/>
-      <c r="E37" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9344,11 +9346,11 @@
         <v>462</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="0" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="F38" s="7"/>
     </row>
@@ -9361,7 +9363,7 @@
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="0" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="F39" s="7"/>
     </row>
@@ -9370,67 +9372,67 @@
         <v>464</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>465</v>
-      </c>
-      <c r="B41" s="9" t="s">
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="9" t="s">
         <v>467</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="B43" s="13" t="s">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>469</v>
       </c>
-      <c r="C43" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="D43" s="13"/>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="13" t="s">
         <v>470</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="D44" s="13"/>
-      <c r="E44" s="0" t="s">
-        <v>176</v>
-      </c>
       <c r="F44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9438,11 +9440,11 @@
         <v>471</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="0" t="s">
-        <v>45</v>
+        <v>176</v>
       </c>
       <c r="F45" s="7"/>
     </row>
@@ -9451,9 +9453,12 @@
         <v>472</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>430</v>
+        <v>34</v>
       </c>
       <c r="D46" s="13"/>
+      <c r="E46" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="F46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9461,12 +9466,9 @@
         <v>473</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="D47" s="13"/>
-      <c r="E47" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9474,11 +9476,11 @@
         <v>474</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="0" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="F48" s="7"/>
     </row>
@@ -9487,9 +9489,12 @@
         <v>475</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D49" s="13"/>
+      <c r="E49" s="0" t="s">
+        <v>79</v>
+      </c>
       <c r="F49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9497,31 +9502,28 @@
         <v>476</v>
       </c>
       <c r="C50" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="0" t="s">
+      <c r="D51" s="13"/>
+      <c r="E51" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>477</v>
-      </c>
-      <c r="B51" s="14" t="s">
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F51" s="7"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="14" t="s">
         <v>479</v>
       </c>
@@ -9552,9 +9554,12 @@
         <v>481</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D54" s="14"/>
+      <c r="E54" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="F54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9562,12 +9567,9 @@
         <v>482</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D55" s="14"/>
-      <c r="E55" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="F55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9575,9 +9577,12 @@
         <v>483</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D56" s="14"/>
+      <c r="E56" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="F56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9595,12 +9600,9 @@
         <v>485</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D58" s="14"/>
-      <c r="E58" s="0" t="s">
-        <v>205</v>
-      </c>
       <c r="F58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9612,46 +9614,46 @@
       </c>
       <c r="D59" s="14"/>
       <c r="E59" s="0" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="14" t="s">
-        <v>141</v>
+        <v>487</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="0" t="s">
-        <v>141</v>
+        <v>210</v>
       </c>
       <c r="F60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="14" t="s">
-        <v>487</v>
+        <v>141</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>488</v>
+        <v>34</v>
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="0" t="s">
-        <v>489</v>
+        <v>141</v>
       </c>
       <c r="F61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="14" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>442</v>
+        <v>489</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="0" t="s">
-        <v>253</v>
+        <v>490</v>
       </c>
       <c r="F62" s="7"/>
     </row>
@@ -9660,11 +9662,11 @@
         <v>491</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="0" t="s">
-        <v>93</v>
+        <v>253</v>
       </c>
       <c r="F63" s="7"/>
     </row>
@@ -9673,9 +9675,12 @@
         <v>492</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D64" s="14"/>
+      <c r="E64" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="F64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9683,12 +9688,9 @@
         <v>493</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>34</v>
+        <v>439</v>
       </c>
       <c r="D65" s="14"/>
-      <c r="E65" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9696,11 +9698,11 @@
         <v>494</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D66" s="14"/>
       <c r="E66" s="0" t="s">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="F66" s="7"/>
     </row>
@@ -9709,9 +9711,12 @@
         <v>495</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D67" s="14"/>
+      <c r="E67" s="0" t="s">
+        <v>192</v>
+      </c>
       <c r="F67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9719,12 +9724,9 @@
         <v>496</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D68" s="14"/>
-      <c r="E68" s="0" t="s">
-        <v>197</v>
-      </c>
       <c r="F68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9732,9 +9734,12 @@
         <v>497</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D69" s="14"/>
+      <c r="E69" s="0" t="s">
+        <v>197</v>
+      </c>
       <c r="F69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9742,12 +9747,9 @@
         <v>498</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>34</v>
+        <v>439</v>
       </c>
       <c r="D70" s="14"/>
-      <c r="E70" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="F70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9755,11 +9757,11 @@
         <v>499</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D71" s="14"/>
       <c r="E71" s="0" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="F71" s="7"/>
     </row>
@@ -9768,9 +9770,12 @@
         <v>500</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D72" s="14"/>
+      <c r="E72" s="0" t="s">
+        <v>125</v>
+      </c>
       <c r="F72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9778,12 +9783,9 @@
         <v>501</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>34</v>
+        <v>439</v>
       </c>
       <c r="D73" s="14"/>
-      <c r="E73" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9795,7 +9797,7 @@
       </c>
       <c r="D74" s="14"/>
       <c r="E74" s="0" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="F74" s="7"/>
     </row>
@@ -9808,7 +9810,7 @@
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="0" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="F75" s="7"/>
     </row>
@@ -9821,7 +9823,7 @@
       </c>
       <c r="D76" s="14"/>
       <c r="E76" s="0" t="s">
-        <v>164</v>
+        <v>45</v>
       </c>
       <c r="F76" s="7"/>
     </row>
@@ -9830,11 +9832,11 @@
         <v>505</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="0" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="F77" s="7"/>
     </row>
@@ -9843,11 +9845,11 @@
         <v>506</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="0" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="F78" s="7"/>
     </row>
@@ -9856,11 +9858,11 @@
         <v>507</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="0" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="F79" s="7"/>
     </row>
@@ -9899,7 +9901,7 @@
       </c>
       <c r="D82" s="14"/>
       <c r="E82" s="0" t="s">
-        <v>160</v>
+        <v>46</v>
       </c>
       <c r="F82" s="7"/>
     </row>
@@ -9912,7 +9914,7 @@
       </c>
       <c r="D83" s="14"/>
       <c r="E83" s="0" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="F83" s="7"/>
     </row>
@@ -9925,7 +9927,7 @@
       </c>
       <c r="D84" s="14"/>
       <c r="E84" s="0" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="F84" s="7"/>
     </row>
@@ -9938,7 +9940,7 @@
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="0" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="F85" s="7"/>
     </row>
@@ -9951,7 +9953,7 @@
       </c>
       <c r="D86" s="14"/>
       <c r="E86" s="0" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="F86" s="7"/>
     </row>
@@ -9960,9 +9962,12 @@
         <v>515</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>430</v>
+        <v>34</v>
       </c>
       <c r="D87" s="14"/>
+      <c r="E87" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="F87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9970,37 +9975,34 @@
         <v>516</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>34</v>
+        <v>430</v>
       </c>
       <c r="D88" s="14"/>
-      <c r="E88" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="14" t="s">
-        <v>240</v>
+        <v>517</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D89" s="14"/>
       <c r="E89" s="0" t="s">
-        <v>240</v>
+        <v>40</v>
       </c>
       <c r="F89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="14" t="s">
-        <v>517</v>
+        <v>240</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="0" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="F90" s="7"/>
     </row>
@@ -10009,11 +10011,11 @@
         <v>518</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D91" s="14"/>
       <c r="E91" s="0" t="s">
-        <v>61</v>
+        <v>234</v>
       </c>
       <c r="F91" s="7"/>
     </row>
@@ -10022,11 +10024,11 @@
         <v>519</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D92" s="14"/>
       <c r="E92" s="0" t="s">
-        <v>229</v>
+        <v>61</v>
       </c>
       <c r="F92" s="7"/>
     </row>
@@ -10039,7 +10041,7 @@
       </c>
       <c r="D93" s="14"/>
       <c r="E93" s="0" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F93" s="7"/>
     </row>
@@ -10048,11 +10050,11 @@
         <v>521</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D94" s="14"/>
       <c r="E94" s="0" t="s">
-        <v>73</v>
+        <v>241</v>
       </c>
       <c r="F94" s="7"/>
     </row>
@@ -10061,37 +10063,37 @@
         <v>522</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D95" s="14"/>
       <c r="E95" s="0" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="F95" s="7"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="14" t="s">
-        <v>242</v>
+        <v>523</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>442</v>
+        <v>34</v>
       </c>
       <c r="D96" s="14"/>
       <c r="E96" s="0" t="s">
-        <v>242</v>
+        <v>42</v>
       </c>
       <c r="F96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="14" t="s">
-        <v>523</v>
+        <v>242</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>34</v>
+        <v>443</v>
       </c>
       <c r="D97" s="14"/>
       <c r="E97" s="0" t="s">
-        <v>48</v>
+        <v>242</v>
       </c>
       <c r="F97" s="7"/>
     </row>
@@ -10100,12 +10102,22 @@
         <v>524</v>
       </c>
       <c r="C98" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D98" s="14"/>
+      <c r="E98" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F98" s="7"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="C99" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="D98" s="14"/>
-      <c r="F98" s="7"/>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D99" s="14"/>
       <c r="F99" s="7"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12084,6 +12096,9 @@
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F758" s="7"/>
+    </row>
+    <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F759" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -12107,7 +12122,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.08203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.09765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.01"/>
@@ -12120,71 +12135,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210305001</v>
+        <v>20210323001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -12192,49 +12207,49 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>

</xml_diff>